<commit_message>
Brand name analyses with logistic regression. Plots reporting proportion of male and female brands
</commit_message>
<xml_diff>
--- a/sk/MergedDataSingleAnalysis.xlsx
+++ b/sk/MergedDataSingleAnalysis.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Samin\Desktop\Machine Learning Project\GenderPrediction\sk\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BCC6090-DF92-4A14-9244-D1BB7ECD90AF}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView activeTab="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Feature</t>
   </si>
@@ -73,23 +79,25 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -104,26 +112,43 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -389,34 +414,36 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="35.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.85546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" s="1" t="n">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="n">
+      <c r="B1" s="1">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="n">
+      <c r="C1" s="1">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="n">
+      <c r="D1" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -430,203 +457,206 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" t="n">
-        <v>0.6524891351362485</v>
-      </c>
-      <c r="C3" t="n">
-        <v>0.9737803865108809</v>
-      </c>
-      <c r="D3" t="n">
-        <v>0.4622032008395645</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
+        <v>13</v>
+      </c>
+      <c r="B3">
+        <v>0.7509423080884019</v>
+      </c>
+      <c r="C3">
+        <v>0.72869483360097453</v>
+      </c>
+      <c r="D3">
+        <v>0.7641184573002755</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4">
+        <v>0.72127247636505942</v>
+      </c>
+      <c r="C4">
+        <v>0.45797109474500253</v>
+      </c>
+      <c r="D4">
+        <v>0.87721369539551353</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>5</v>
       </c>
-      <c r="B4" t="n">
-        <v>0.6606867005828923</v>
-      </c>
-      <c r="C4" t="n">
+      <c r="B5">
+        <v>0.66068670058289225</v>
+      </c>
+      <c r="C5">
         <v>0.1176698599036491</v>
       </c>
-      <c r="D4" t="n">
-        <v>0.9822904368358913</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" t="n">
-        <v>0.7212724763650594</v>
-      </c>
-      <c r="C5" t="n">
-        <v>0.4579710947450025</v>
-      </c>
-      <c r="D5" t="n">
-        <v>0.8772136953955135</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
+      <c r="D5">
+        <v>0.98229043683589135</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
-      <c r="B6" t="n">
-        <v>0.6582665650553027</v>
-      </c>
-      <c r="C6" t="n">
-        <v>0.1224043413256548</v>
-      </c>
-      <c r="D6" t="n">
+      <c r="B6">
+        <v>0.65826656505530268</v>
+      </c>
+      <c r="C6">
+        <v>0.12240434132565479</v>
+      </c>
+      <c r="D6">
         <v>0.9756329529056802</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7">
+        <v>0.65248913513624851</v>
+      </c>
+      <c r="C7">
+        <v>0.97378038651088095</v>
+      </c>
+      <c r="D7">
+        <v>0.46220320083956451</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8">
+        <v>0.63383864390022859</v>
+      </c>
+      <c r="C8">
+        <v>8.8570795725123205E-2</v>
+      </c>
+      <c r="D8">
+        <v>0.95677554768463857</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9">
+        <v>0.63070791538794257</v>
+      </c>
+      <c r="C9">
+        <v>1.7138269007143249E-2</v>
+      </c>
+      <c r="D9">
+        <v>0.99409681227863045</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10">
+        <v>0.6284422565961566</v>
+      </c>
+      <c r="C10">
+        <v>1.4120383188437899E-3</v>
+      </c>
+      <c r="D10">
+        <v>0.99980322707595437</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>8</v>
       </c>
-      <c r="B7" t="n">
-        <v>0.6280406170830672</v>
-      </c>
-      <c r="C7" t="n">
+      <c r="B11">
+        <v>0.62804061708306724</v>
+      </c>
+      <c r="C11">
         <v>0</v>
       </c>
-      <c r="D7" t="n">
+      <c r="D11">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
-      <c r="A8" t="s">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>9</v>
       </c>
-      <c r="B8" t="n">
-        <v>0.6280406170830672</v>
-      </c>
-      <c r="C8" t="n">
+      <c r="B12">
+        <v>0.62804061708306724</v>
+      </c>
+      <c r="C12">
         <v>0</v>
       </c>
-      <c r="D8" t="n">
+      <c r="D12">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
-      <c r="A9" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9" t="n">
-        <v>0.6338386439002286</v>
-      </c>
-      <c r="C9" t="n">
-        <v>0.08857079572512321</v>
-      </c>
-      <c r="D9" t="n">
-        <v>0.9567755476846386</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10" t="s">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>11</v>
       </c>
-      <c r="B10" t="n">
-        <v>0.6280406170830672</v>
-      </c>
-      <c r="C10" t="n">
+      <c r="B13">
+        <v>0.62804061708306724</v>
+      </c>
+      <c r="C13">
         <v>0</v>
       </c>
-      <c r="D10" t="n">
+      <c r="D13">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
-      <c r="A11" t="s">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14">
+        <v>0.62804061708306724</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15">
+        <v>0.62804061708306724</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>12</v>
       </c>
-      <c r="B11" t="n">
-        <v>0.6263001791930135</v>
-      </c>
-      <c r="C11" t="n">
-        <v>0.02461376598925744</v>
-      </c>
-      <c r="D11" t="n">
+      <c r="B16">
+        <v>0.62630017919301351</v>
+      </c>
+      <c r="C16">
+        <v>2.4613765989257439E-2</v>
+      </c>
+      <c r="D16">
         <v>0.9826511871966418</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
-      <c r="A12" t="s">
-        <v>13</v>
-      </c>
-      <c r="B12" t="n">
-        <v>0.7509423080884019</v>
-      </c>
-      <c r="C12" t="n">
-        <v>0.7286948336009745</v>
-      </c>
-      <c r="D12" t="n">
-        <v>0.7641184573002755</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
-      <c r="A13" t="s">
-        <v>14</v>
-      </c>
-      <c r="B13" t="n">
-        <v>0.6307079153879426</v>
-      </c>
-      <c r="C13" t="n">
-        <v>0.01713826900714325</v>
-      </c>
-      <c r="D13" t="n">
-        <v>0.9940968122786304</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4">
-      <c r="A14" t="s">
-        <v>15</v>
-      </c>
-      <c r="B14" t="n">
-        <v>0.6284422565961566</v>
-      </c>
-      <c r="C14" t="n">
-        <v>0.00141203831884379</v>
-      </c>
-      <c r="D14" t="n">
-        <v>0.9998032270759544</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4">
-      <c r="A15" t="s">
-        <v>16</v>
-      </c>
-      <c r="B15" t="n">
-        <v>0.6280406170830672</v>
-      </c>
-      <c r="C15" t="n">
-        <v>0</v>
-      </c>
-      <c r="D15" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4">
-      <c r="A16" t="s">
-        <v>17</v>
-      </c>
-      <c r="B16" t="n">
-        <v>0.6280406170830672</v>
-      </c>
-      <c r="C16" t="n">
-        <v>0</v>
-      </c>
-      <c r="D16" t="n">
-        <v>1</v>
-      </c>
-    </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <sortState ref="A2:D16">
+    <sortCondition descending="1" ref="B1"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>